<commit_message>
able to read write
</commit_message>
<xml_diff>
--- a/1.Document/Communication Example (Exel)/Example comunication frame.xlsx
+++ b/1.Document/Communication Example (Exel)/Example comunication frame.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -364,7 +364,7 @@
   <dimension ref="B4:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>